<commit_message>
Same random fixes & clean ups
</commit_message>
<xml_diff>
--- a/objects_in_task.xlsx
+++ b/objects_in_task.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Work\researchProjects\OLM_project\experiment\unityProjects\Object-Location-Memory-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590E84F6-8419-4EF8-AD9D-E5671EE5F386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67331E98-D041-45CB-A568-DA5CD9778F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="144" yWindow="1104" windowWidth="17280" windowHeight="8964" xr2:uid="{33EF67CF-700A-4369-ADA7-BFA23192FEF1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33EF67CF-700A-4369-ADA7-BFA23192FEF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="117">
   <si>
     <t>Drum</t>
   </si>
@@ -237,6 +237,156 @@
   </si>
   <si>
     <t>Harmonica</t>
+  </si>
+  <si>
+    <t>Classical/categorical</t>
+  </si>
+  <si>
+    <t>Internal name</t>
+  </si>
+  <si>
+    <t>barrel</t>
+  </si>
+  <si>
+    <t>basketball</t>
+  </si>
+  <si>
+    <t>cake</t>
+  </si>
+  <si>
+    <t>dice</t>
+  </si>
+  <si>
+    <t>donut</t>
+  </si>
+  <si>
+    <t>drum</t>
+  </si>
+  <si>
+    <t>football</t>
+  </si>
+  <si>
+    <t>gift</t>
+  </si>
+  <si>
+    <t>lamp</t>
+  </si>
+  <si>
+    <t>pawn</t>
+  </si>
+  <si>
+    <t>pineapple</t>
+  </si>
+  <si>
+    <t>vase</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>chimpanzee</t>
+  </si>
+  <si>
+    <t>clarinet</t>
+  </si>
+  <si>
+    <t>deer</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>drill</t>
+  </si>
+  <si>
+    <t>elephant</t>
+  </si>
+  <si>
+    <t>guitar</t>
+  </si>
+  <si>
+    <t>hammer</t>
+  </si>
+  <si>
+    <t>harmonica</t>
+  </si>
+  <si>
+    <t>hippo</t>
+  </si>
+  <si>
+    <t>kangaroo</t>
+  </si>
+  <si>
+    <t>lemon</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>pear</t>
+  </si>
+  <si>
+    <t>piano</t>
+  </si>
+  <si>
+    <t>pliers</t>
+  </si>
+  <si>
+    <t>pomegranate</t>
+  </si>
+  <si>
+    <t>saw</t>
+  </si>
+  <si>
+    <t>saxophone</t>
+  </si>
+  <si>
+    <t>strawberry</t>
+  </si>
+  <si>
+    <t>tiger</t>
+  </si>
+  <si>
+    <t>trumpet</t>
+  </si>
+  <si>
+    <t>turnscrew</t>
+  </si>
+  <si>
+    <t>violin</t>
+  </si>
+  <si>
+    <t>watermelon</t>
+  </si>
+  <si>
+    <t>wrench</t>
+  </si>
+  <si>
+    <t>zebra</t>
+  </si>
+  <si>
+    <t>cone</t>
+  </si>
+  <si>
+    <t>teddy</t>
+  </si>
+  <si>
+    <t>keyboard</t>
+  </si>
+  <si>
+    <t>cutter_knife</t>
+  </si>
+  <si>
+    <t>insulating_tape</t>
+  </si>
+  <si>
+    <t>measurement_tape</t>
+  </si>
+  <si>
+    <t>polar_bear</t>
   </si>
 </sst>
 </file>
@@ -594,866 +744,1013 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BAFAFA9-8A3A-4982-B28D-C4B3D2F75CAA}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="25.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>58</v>
       </c>
       <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>62</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>50</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>50</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>50</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>50</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
       <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
         <v>65</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>50</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>50</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
       <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
         <v>53</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>50</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>17</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>51</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
-        <v>52</v>
-      </c>
       <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
         <v>53</v>
       </c>
-      <c r="F16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17">
         <v>16</v>
       </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
       <c r="E17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" t="s">
         <v>53</v>
       </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18">
         <v>17</v>
       </c>
-      <c r="D18" t="s">
-        <v>52</v>
-      </c>
       <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
         <v>54</v>
       </c>
-      <c r="F18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19">
         <v>18</v>
       </c>
-      <c r="D19" t="s">
-        <v>52</v>
-      </c>
       <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" t="s">
         <v>65</v>
       </c>
-      <c r="F19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20">
         <v>19</v>
       </c>
-      <c r="D20" t="s">
-        <v>52</v>
-      </c>
       <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" t="s">
         <v>56</v>
       </c>
-      <c r="F20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21" t="s">
-        <v>52</v>
-      </c>
       <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" t="s">
         <v>54</v>
       </c>
-      <c r="F21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22">
         <v>21</v>
       </c>
-      <c r="D22" t="s">
-        <v>52</v>
-      </c>
       <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" t="s">
         <v>54</v>
       </c>
-      <c r="F22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
-        <v>52</v>
-      </c>
       <c r="E23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" t="s">
         <v>56</v>
       </c>
-      <c r="F23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24">
         <v>23</v>
       </c>
-      <c r="D24" t="s">
-        <v>52</v>
-      </c>
       <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
         <v>54</v>
       </c>
-      <c r="F24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25">
         <v>24</v>
       </c>
-      <c r="D25" t="s">
-        <v>52</v>
-      </c>
       <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
         <v>65</v>
       </c>
-      <c r="F25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26">
         <v>25</v>
       </c>
-      <c r="D26" t="s">
-        <v>52</v>
-      </c>
       <c r="E26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" t="s">
         <v>56</v>
       </c>
-      <c r="F26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>66</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27">
         <v>26</v>
       </c>
-      <c r="D27" t="s">
-        <v>52</v>
-      </c>
       <c r="E27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" t="s">
         <v>65</v>
       </c>
-      <c r="F27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28">
         <v>27</v>
       </c>
-      <c r="D28" t="s">
-        <v>52</v>
-      </c>
       <c r="E28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" t="s">
         <v>54</v>
       </c>
-      <c r="F28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29">
         <v>28</v>
       </c>
-      <c r="D29" t="s">
-        <v>52</v>
-      </c>
       <c r="E29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" t="s">
         <v>56</v>
       </c>
-      <c r="F29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30">
         <v>29</v>
       </c>
-      <c r="D30" t="s">
-        <v>52</v>
-      </c>
       <c r="E30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" t="s">
         <v>54</v>
       </c>
-      <c r="F30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31">
         <v>30</v>
       </c>
-      <c r="D31" t="s">
-        <v>52</v>
-      </c>
       <c r="E31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" t="s">
         <v>65</v>
       </c>
-      <c r="F31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32">
         <v>31</v>
       </c>
-      <c r="D32" t="s">
-        <v>52</v>
-      </c>
       <c r="E32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" t="s">
         <v>53</v>
       </c>
-      <c r="F32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33">
         <v>32</v>
       </c>
-      <c r="D33" t="s">
-        <v>52</v>
-      </c>
       <c r="E33" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" t="s">
         <v>56</v>
       </c>
-      <c r="F33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34">
         <v>33</v>
       </c>
-      <c r="D34" t="s">
-        <v>52</v>
-      </c>
       <c r="E34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" t="s">
         <v>53</v>
       </c>
-      <c r="F34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35">
         <v>34</v>
       </c>
-      <c r="D35" t="s">
-        <v>52</v>
-      </c>
       <c r="E35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" t="s">
         <v>53</v>
       </c>
-      <c r="F35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36">
         <v>35</v>
       </c>
-      <c r="D36" t="s">
-        <v>52</v>
-      </c>
       <c r="E36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" t="s">
         <v>65</v>
       </c>
-      <c r="F36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37">
         <v>36</v>
       </c>
-      <c r="D37" t="s">
-        <v>52</v>
-      </c>
       <c r="E37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" t="s">
         <v>56</v>
       </c>
-      <c r="F37" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38">
         <v>37</v>
       </c>
-      <c r="D38" t="s">
-        <v>52</v>
-      </c>
       <c r="E38" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" t="s">
         <v>54</v>
       </c>
-      <c r="F38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="B39">
+      <c r="B39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39">
         <v>38</v>
       </c>
-      <c r="D39" t="s">
-        <v>52</v>
-      </c>
       <c r="E39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" t="s">
         <v>53</v>
       </c>
-      <c r="F39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40">
         <v>39</v>
       </c>
-      <c r="D40" t="s">
-        <v>52</v>
-      </c>
       <c r="E40" t="s">
+        <v>52</v>
+      </c>
+      <c r="F40" t="s">
         <v>56</v>
       </c>
-      <c r="F40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
-      <c r="B41">
+      <c r="B41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41">
         <v>40</v>
       </c>
-      <c r="D41" t="s">
-        <v>52</v>
-      </c>
       <c r="E41" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" t="s">
         <v>65</v>
       </c>
-      <c r="F41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
-      <c r="B42">
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42">
         <v>41</v>
       </c>
-      <c r="D42" t="s">
-        <v>52</v>
-      </c>
       <c r="E42" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" t="s">
         <v>53</v>
       </c>
-      <c r="F42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="B43">
+      <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43">
         <v>42</v>
       </c>
-      <c r="D43" t="s">
-        <v>52</v>
-      </c>
       <c r="E43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" t="s">
         <v>54</v>
       </c>
-      <c r="F43" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>57</v>
       </c>
-      <c r="B44">
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44">
         <v>43</v>
       </c>
-      <c r="D44" t="s">
-        <v>52</v>
-      </c>
       <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" t="s">
         <v>65</v>
       </c>
-      <c r="F44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>45</v>
       </c>
-      <c r="B45">
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45">
         <v>44</v>
       </c>
-      <c r="D45" t="s">
-        <v>52</v>
-      </c>
       <c r="E45" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" t="s">
         <v>56</v>
       </c>
-      <c r="F45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
-      <c r="B46">
+      <c r="B46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46">
         <v>45</v>
       </c>
-      <c r="D46" t="s">
-        <v>52</v>
-      </c>
       <c r="E46" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" t="s">
         <v>65</v>
       </c>
-      <c r="F46" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
-      <c r="B47">
+      <c r="B47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47">
         <v>46</v>
       </c>
-      <c r="D47" t="s">
-        <v>52</v>
-      </c>
       <c r="E47" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" t="s">
         <v>53</v>
       </c>
-      <c r="F47" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>48</v>
       </c>
-      <c r="B48">
+      <c r="B48" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48">
         <v>47</v>
       </c>
-      <c r="D48" t="s">
-        <v>52</v>
-      </c>
       <c r="E48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F48" t="s">
         <v>56</v>
       </c>
-      <c r="F48" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>49</v>
       </c>
-      <c r="B49">
+      <c r="B49" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49">
         <v>48</v>
       </c>
-      <c r="D49" t="s">
-        <v>52</v>
-      </c>
       <c r="E49" t="s">
+        <v>52</v>
+      </c>
+      <c r="F49" t="s">
         <v>54</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C15">
-    <sortCondition ref="B2:B15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D15">
+    <sortCondition ref="C2:C15"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>